<commit_message>
added electrified driving time calculation
</commit_message>
<xml_diff>
--- a/Route_Description/Apeldoorn_Zutphun.xlsx
+++ b/Route_Description/Apeldoorn_Zutphun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Documents\0_Robotics\EVSD\Python\Route_Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5F6B97-231B-4661-B51B-FB5458DC14A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DD1CDD-3C12-43B6-B865-9366F4DBDF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>Stop electrification</t>
   </si>
   <si>
-    <t>Stop time (min)</t>
-  </si>
-  <si>
     <t>speed limit</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Stop time</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,18 +415,18 @@
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -443,7 +443,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -511,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -580,13 +580,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>